<commit_message>
Common: Preparing the big show of the Excel reading
</commit_message>
<xml_diff>
--- a/tests/Edde/fixtures/complex-import.xlsx
+++ b/tests/Edde/fixtures/complex-import.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\leight-core\edde\tests\Edde\Import\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\leight-core\edde\tests\Edde\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E91605-1DC1-4E87-81B5-924314C0D931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D997CD63-683A-4C4B-BBEE-0B50A6E267D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="9120" windowWidth="46260" windowHeight="12210" activeTab="6" xr2:uid="{4F598108-ABED-4A15-AA0A-0BA5C2D2ACC7}"/>
+    <workbookView xWindow="22890" yWindow="9720" windowWidth="26085" windowHeight="8880" xr2:uid="{4F598108-ABED-4A15-AA0A-0BA5C2D2ACC7}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -489,9 +489,6 @@
     <t>tab</t>
   </si>
   <si>
-    <t>service</t>
-  </si>
-  <si>
     <t>Edde\Import\SomeImporter, Edde\Import\OverlapImporter</t>
   </si>
   <si>
@@ -523,6 +520,9 @@
   </si>
   <si>
     <t>Poslední import - překlady</t>
+  </si>
+  <si>
+    <t>services</t>
   </si>
 </sst>
 </file>
@@ -905,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80400769-8F00-40E1-AEF6-B36AA409EFC7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +920,7 @@
         <v>147</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1036,34 +1036,34 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
         <v>152</v>
-      </c>
-      <c r="B3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
         <v>156</v>
-      </c>
-      <c r="B4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" t="s">
         <v>158</v>
-      </c>
-      <c r="B5" t="s">
-        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A618FB-AA69-43D3-BC82-4EF0EA69614C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1710,7 +1710,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Some fun with reflection and readers/importers
</commit_message>
<xml_diff>
--- a/tests/Edde/fixtures/complex-import.xlsx
+++ b/tests/Edde/fixtures/complex-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\leight-core\edde\tests\Edde\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D997CD63-683A-4C4B-BBEE-0B50A6E267D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB7821A-DAC4-4114-9C47-DFF6AAFB6C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22890" yWindow="9720" windowWidth="26085" windowHeight="8880" xr2:uid="{4F598108-ABED-4A15-AA0A-0BA5C2D2ACC7}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="161">
   <si>
     <t>Nějaký import</t>
   </si>
@@ -477,30 +477,12 @@
     <t>An Empty Page</t>
   </si>
   <si>
-    <t>Edde\Import\AnotherImporter</t>
-  </si>
-  <si>
-    <t>Edde\Import\EmptyPageImporter</t>
-  </si>
-  <si>
-    <t>Edde\Import\LastManStandingImporter</t>
-  </si>
-  <si>
     <t>tab</t>
   </si>
   <si>
-    <t>Edde\Import\SomeImporter, Edde\Import\OverlapImporter</t>
-  </si>
-  <si>
     <t>Nějaký import - překlady</t>
   </si>
   <si>
-    <t>Edde\Import\SomeImporter.translations</t>
-  </si>
-  <si>
-    <t>Edde\Import\OverlapImporter.translations</t>
-  </si>
-  <si>
     <t>Překryv - překlady</t>
   </si>
   <si>
@@ -510,19 +492,40 @@
     <t>bar</t>
   </si>
   <si>
-    <t>Edde\Import\AnotherImporter.translations</t>
-  </si>
-  <si>
     <t>Další import - překlady</t>
   </si>
   <si>
-    <t>Edde\Import\LastManStandingImporter.translations</t>
-  </si>
-  <si>
     <t>Poslední import - překlady</t>
   </si>
   <si>
     <t>services</t>
+  </si>
+  <si>
+    <t>Bad one</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\SomeImporter.translations</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\OverlapImporter.translations</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\AnotherImporter.translations</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\LastManStandingImporter.translations</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\SomeImporter, Edde\Import\Importer\OverlapImporter</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\AnotherImporter</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\LastManStandingImporter</t>
+  </si>
+  <si>
+    <t>Edde\Import\Importer\EmptyPageImporter</t>
   </si>
 </sst>
 </file>
@@ -906,21 +909,21 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -928,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -936,7 +939,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -944,7 +947,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -952,7 +955,7 @@
         <v>143</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -965,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565791B0-C2EA-4A38-B5A1-1BB3A6800ECB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -1017,12 +1020,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="58.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1036,18 +1039,18 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,15 +1058,15 @@
         <v>155</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1073,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC388F06-1610-4B97-A25E-F057892E2064}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,6 +1318,11 @@
       </c>
       <c r="C21" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1637,7 +1645,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1718,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1718,7 +1726,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Moved DTO resolution to another place
</commit_message>
<xml_diff>
--- a/tests/Edde/fixtures/complex-import.xlsx
+++ b/tests/Edde/fixtures/complex-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\leight-core\edde\tests\Edde\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB7821A-DAC4-4114-9C47-DFF6AAFB6C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2262BC51-1B16-46A7-921F-E64744072A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22890" yWindow="9720" windowWidth="26085" windowHeight="8880" xr2:uid="{4F598108-ABED-4A15-AA0A-0BA5C2D2ACC7}"/>
+    <workbookView xWindow="22890" yWindow="9720" windowWidth="26085" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{4F598108-ABED-4A15-AA0A-0BA5C2D2ACC7}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="158">
   <si>
     <t>Nějaký import</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Some value 020</t>
   </si>
   <si>
-    <t>Another Value 001</t>
-  </si>
-  <si>
     <t>Another Value 002</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>Another Value 020</t>
   </si>
   <si>
-    <t>Va-Va-Value 001</t>
-  </si>
-  <si>
     <t>Va-Va-Value 002</t>
   </si>
   <si>
@@ -499,9 +493,6 @@
   </si>
   <si>
     <t>services</t>
-  </si>
-  <si>
-    <t>Bad one</t>
   </si>
   <si>
     <t>Edde\Import\Importer\SomeImporter.translations</t>
@@ -908,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80400769-8F00-40E1-AEF6-B36AA409EFC7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,10 +911,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -931,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +930,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,15 +938,15 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1039,34 +1030,34 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1076,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC388F06-1610-4B97-A25E-F057892E2064}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,22 +1095,16 @@
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,10 +1112,10 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,10 +1123,10 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1149,10 +1134,10 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,10 +1145,10 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1171,10 +1156,10 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1182,10 +1167,10 @@
         <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,10 +1178,10 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,10 +1189,10 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,10 +1200,10 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,10 +1211,10 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,10 +1222,10 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,10 +1233,10 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,10 +1244,10 @@
         <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,10 +1255,10 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,10 +1266,10 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,10 +1277,10 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1303,10 +1288,10 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1314,15 +1299,10 @@
         <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1359,68 +1339,68 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
         <v>95</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1471,167 +1451,167 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" t="s">
         <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
         <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" t="s">
         <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
         <v>113</v>
-      </c>
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
         <v>116</v>
-      </c>
-      <c r="B8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
         <v>119</v>
-      </c>
-      <c r="B9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
         <v>122</v>
-      </c>
-      <c r="B10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
         <v>125</v>
-      </c>
-      <c r="B11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
         <v>131</v>
-      </c>
-      <c r="B13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
         <v>134</v>
-      </c>
-      <c r="B14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" t="s">
         <v>137</v>
-      </c>
-      <c r="B15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C15" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C16" t="s">
         <v>140</v>
-      </c>
-      <c r="B16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C16" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1718,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1726,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>